<commit_message>
Fix a bug in excel file and in backup.sql file
</commit_message>
<xml_diff>
--- a/tests/test_excel.xlsx
+++ b/tests/test_excel.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="32">
   <si>
     <t>YEAR</t>
   </si>
@@ -96,6 +96,15 @@
   </si>
   <si>
     <t>משכורת</t>
+  </si>
+  <si>
+    <t>מכון כושר</t>
+  </si>
+  <si>
+    <t>מועדון</t>
+  </si>
+  <si>
+    <t>בית</t>
   </si>
   <si>
     <t>סה״כ</t>
@@ -232,23 +241,41 @@
           </c:tx>
           <c:cat>
             <c:strRef>
-              <c:f>YEAR!$A$19</c:f>
+              <c:f>YEAR!$A$19:$A$22</c:f>
               <c:strCache>
-                <c:ptCount val="1"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
+                  <c:v>מכון כושר</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>מועדון</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>אוכל</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>בית</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>YEAR!$C$19</c:f>
+              <c:f>YEAR!$C$19:$C$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>230</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -314,7 +341,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>YEAR!$B$4:$M$4</c:f>
+              <c:f>YEAR!$B$34:$M$34</c:f>
               <c:strCache>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
@@ -358,7 +385,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>YEAR!$B$5:$M$5</c:f>
+              <c:f>YEAR!$B$37:$M$37</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -366,7 +393,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -453,6 +480,1259 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
+                  <a:t>סה״כ חסכון</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="50100001"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>YEAR!$B$34:$M$34</c:f>
+              <c:strCache>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>JAN</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>FEB</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>MAR</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>APR</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>MAY</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>JUN</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>JUL</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>AUG</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>SEP</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>OCT</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>NOV</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>DEC</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>YEAR!$B$36:$M$36</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:marker val="1"/>
+        <c:axId val="50110001"/>
+        <c:axId val="50110002"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="50110001"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Months</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="50110002"/>
+        <c:crosses val="autoZero"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="50110002"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>סה״כ הוצאות</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="50110001"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>YEAR!$B$34:$M$34</c:f>
+              <c:strCache>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>JAN</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>FEB</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>MAR</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>APR</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>MAY</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>JUN</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>JUL</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>AUG</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>SEP</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>OCT</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>NOV</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>DEC</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>YEAR!$B$35:$M$35</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:marker val="1"/>
+        <c:axId val="50120001"/>
+        <c:axId val="50120002"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="50120001"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Months</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="50120002"/>
+        <c:crosses val="autoZero"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="50120002"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>סה״כ הכנסות</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="50120001"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart13.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>YEAR!$B$18:$M$18</c:f>
+              <c:strCache>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>JAN</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>FEB</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>MAR</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>APR</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>MAY</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>JUN</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>JUL</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>AUG</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>SEP</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>OCT</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>NOV</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>DEC</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>YEAR!$B$22:$M$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>540</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:marker val="1"/>
+        <c:axId val="50130001"/>
+        <c:axId val="50130002"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="50130001"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Months</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="50130002"/>
+        <c:crosses val="autoZero"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="50130002"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>בית</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="50130001"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart14.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>YEAR!$B$18:$M$18</c:f>
+              <c:strCache>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>JAN</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>FEB</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>MAR</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>APR</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>MAY</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>JUN</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>JUL</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>AUG</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>SEP</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>OCT</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>NOV</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>DEC</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>YEAR!$B$21:$M$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>230</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>230</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>230</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:marker val="1"/>
+        <c:axId val="50140001"/>
+        <c:axId val="50140002"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="50140001"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Months</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="50140002"/>
+        <c:crosses val="autoZero"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="50140002"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>אוכל</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="50140001"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart15.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>YEAR!$B$18:$M$18</c:f>
+              <c:strCache>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>JAN</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>FEB</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>MAR</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>APR</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>MAY</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>JUN</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>JUL</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>AUG</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>SEP</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>OCT</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>NOV</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>DEC</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>YEAR!$B$20:$M$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:marker val="1"/>
+        <c:axId val="50150001"/>
+        <c:axId val="50150002"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="50150001"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Months</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="50150002"/>
+        <c:crosses val="autoZero"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="50150002"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>מועדון</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="50150001"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart16.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>YEAR!$B$18:$M$18</c:f>
+              <c:strCache>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>JAN</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>FEB</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>MAR</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>APR</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>MAY</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>JUN</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>JUL</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>AUG</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>SEP</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>OCT</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>NOV</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>DEC</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>YEAR!$B$19:$M$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>520</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:marker val="1"/>
+        <c:axId val="50160001"/>
+        <c:axId val="50160002"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="50160001"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Months</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="50160002"/>
+        <c:crosses val="autoZero"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="50160002"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>מכון כושר</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="50160001"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart17.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>YEAR!$B$4:$M$4</c:f>
+              <c:strCache>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>JAN</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>FEB</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>MAR</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>APR</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>MAY</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>JUN</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>JUL</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>AUG</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>SEP</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>OCT</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>NOV</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>DEC</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>YEAR!$B$5:$M$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:marker val="1"/>
+        <c:axId val="50170001"/>
+        <c:axId val="50170002"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="50170001"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Months</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="50170002"/>
+        <c:crosses val="autoZero"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="50170002"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
                   <a:t>משכורת</a:t>
                 </a:r>
               </a:p>
@@ -462,7 +1742,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="50100001"/>
+        <c:crossAx val="50170001"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -593,146 +1873,70 @@
   <c:chart>
     <c:plotArea>
       <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:strRef>
-              <c:f>YEAR!$A$5</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>משכורת</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+            <c:v>סה״כ הוצאות לפי נושא</c:v>
           </c:tx>
-          <c:marker>
-            <c:symbol val="circle"/>
-          </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>YEAR!$B$4:$M$4</c:f>
+              <c:f>YEAR!$A$19:$A$22</c:f>
               <c:strCache>
-                <c:ptCount val="12"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>JAN</c:v>
+                  <c:v>מכון כושר</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>FEB</c:v>
+                  <c:v>מועדון</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>MAR</c:v>
+                  <c:v>אוכל</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>APR</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>MAY</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>JUN</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>JUL</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>AUG</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>SEP</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>OCT</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>NOV</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>DEC</c:v>
+                  <c:v>בית</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>YEAR!$B$5:$M$5</c:f>
+              <c:f>YEAR!$D$19:$D$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>230</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="11">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:marker val="1"/>
         <c:axId val="50030001"/>
         <c:axId val="50030002"/>
-      </c:lineChart>
+      </c:barChart>
       <c:catAx>
         <c:axId val="50030001"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Months</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout/>
-        </c:title>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="50030002"/>
         <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
@@ -742,31 +1946,18 @@
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="l"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000" vert="horz"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>הכנסות לפי חודש</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout/>
-        </c:title>
+        <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="50030001"/>
         <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
+        <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
@@ -783,146 +1974,79 @@
   <c:chart>
     <c:plotArea>
       <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:strRef>
-              <c:f>YEAR!$A$19</c:f>
-              <c:strCache>
+            <c:v>סה״כ הוצאות</c:v>
+          </c:tx>
+          <c:val>
+            <c:numRef>
+              <c:f>MAR!$B$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>אוכל</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:marker>
-            <c:symbol val="circle"/>
-          </c:marker>
-          <c:cat>
-            <c:strRef>
-              <c:f>YEAR!$B$18:$M$18</c:f>
-              <c:strCache>
-                <c:ptCount val="12"/>
-                <c:pt idx="0">
-                  <c:v>JAN</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>FEB</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>MAR</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>APR</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>MAY</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>JUN</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>JUL</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>AUG</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>SEP</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>OCT</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>NOV</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>DEC</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>YEAR!$B$19:$M$19</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>230</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="11">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:marker val="1"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>סה״כ הכנסות</c:v>
+          </c:tx>
+          <c:val>
+            <c:numRef>
+              <c:f>MAR!$I$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>סה״כ חיסכון</c:v>
+          </c:tx>
+          <c:val>
+            <c:numRef>
+              <c:f>MAR!$I$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
         <c:axId val="50040001"/>
         <c:axId val="50040002"/>
-      </c:lineChart>
+      </c:barChart>
       <c:catAx>
         <c:axId val="50040001"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Months</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout/>
-        </c:title>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="50040002"/>
         <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
@@ -932,31 +2056,18 @@
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="l"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000" vert="horz"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>הוצאות לפי חודש</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout/>
-        </c:title>
+        <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="50040001"/>
         <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
+        <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
@@ -973,135 +2084,70 @@
   <c:chart>
     <c:plotArea>
       <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
+          <c:tx>
+            <c:v>סה״כ הוצאות לפי נושא</c:v>
+          </c:tx>
           <c:cat>
             <c:strRef>
-              <c:f>YEAR!$B$31:$M$31</c:f>
+              <c:f>YEAR!$A$19:$A$22</c:f>
               <c:strCache>
-                <c:ptCount val="12"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>JAN</c:v>
+                  <c:v>מכון כושר</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>FEB</c:v>
+                  <c:v>מועדון</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>MAR</c:v>
+                  <c:v>אוכל</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>APR</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>MAY</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>JUN</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>JUL</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>AUG</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>SEP</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>OCT</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>NOV</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>DEC</c:v>
+                  <c:v>בית</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>YEAR!$B$35:$M$35</c:f>
+              <c:f>YEAR!$E$19:$E$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>520</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>230</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0</c:v>
+                  <c:v>540</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:marker val="1"/>
         <c:axId val="50050001"/>
         <c:axId val="50050002"/>
-      </c:lineChart>
+      </c:barChart>
       <c:catAx>
         <c:axId val="50050001"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Months</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout/>
-        </c:title>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="50050002"/>
         <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
@@ -1111,31 +2157,18 @@
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="l"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000" vert="horz"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>אחוז חיסכון</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout/>
-        </c:title>
+        <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="50050001"/>
         <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
+        <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
@@ -1152,135 +2185,79 @@
   <c:chart>
     <c:plotArea>
       <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:strRef>
-              <c:f>YEAR!$B$31:$M$31</c:f>
-              <c:strCache>
-                <c:ptCount val="12"/>
-                <c:pt idx="0">
-                  <c:v>JAN</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>FEB</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>MAR</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>APR</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>MAY</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>JUN</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>JUL</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>AUG</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>SEP</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>OCT</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>NOV</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>DEC</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
+          <c:tx>
+            <c:v>סה״כ הוצאות</c:v>
+          </c:tx>
           <c:val>
             <c:numRef>
-              <c:f>YEAR!$B$34:$M$34</c:f>
+              <c:f>APR!$B$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="11">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:marker val="1"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>סה״כ הכנסות</c:v>
+          </c:tx>
+          <c:val>
+            <c:numRef>
+              <c:f>APR!$I$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>סה״כ חיסכון</c:v>
+          </c:tx>
+          <c:val>
+            <c:numRef>
+              <c:f>APR!$I$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
         <c:axId val="50060001"/>
         <c:axId val="50060002"/>
-      </c:lineChart>
+      </c:barChart>
       <c:catAx>
         <c:axId val="50060001"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Months</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout/>
-        </c:title>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="50060002"/>
         <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
@@ -1290,31 +2267,18 @@
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="l"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000" vert="horz"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>סה״כ חסכון</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout/>
-        </c:title>
+        <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="50060001"/>
         <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
+        <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
@@ -1336,12 +2300,23 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>YEAR!$A$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>משכורת</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="circle"/>
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>YEAR!$B$31:$M$31</c:f>
+              <c:f>YEAR!$B$4:$M$4</c:f>
               <c:strCache>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
@@ -1385,7 +2360,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>YEAR!$B$33:$M$33</c:f>
+              <c:f>YEAR!$B$5:$M$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -1393,13 +2368,13 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>5000</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>4000</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>6000</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -1480,7 +2455,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>סה״כ הוצאות</a:t>
+                  <a:t>הכנסות לפי חודש</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -1515,12 +2490,23 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>YEAR!$A$19</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>מכון כושר</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="circle"/>
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>YEAR!$B$31:$M$31</c:f>
+              <c:f>YEAR!$B$18:$M$18</c:f>
               <c:strCache>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
@@ -1564,7 +2550,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>YEAR!$B$32:$M$32</c:f>
+              <c:f>YEAR!$B$19:$M$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -1578,7 +2564,328 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>520</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>YEAR!$A$20</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>מועדון</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="circle"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>YEAR!$B$18:$M$18</c:f>
+              <c:strCache>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>JAN</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>FEB</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>MAR</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>APR</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>MAY</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>JUN</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>JUL</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>AUG</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>SEP</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>OCT</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>NOV</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>DEC</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>YEAR!$B$20:$M$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>YEAR!$A$21</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>אוכל</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="circle"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>YEAR!$B$18:$M$18</c:f>
+              <c:strCache>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>JAN</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>FEB</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>MAR</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>APR</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>MAY</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>JUN</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>JUL</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>AUG</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>SEP</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>OCT</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>NOV</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>DEC</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>YEAR!$B$21:$M$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>230</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>230</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>230</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>YEAR!$A$22</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>בית</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="circle"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>YEAR!$B$18:$M$18</c:f>
+              <c:strCache>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>JAN</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>FEB</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>MAR</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>APR</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>MAY</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>JUN</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>JUL</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>AUG</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>SEP</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>OCT</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>NOV</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>DEC</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>YEAR!$B$22:$M$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>540</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -1659,7 +2966,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>סה״כ הכנסות</a:t>
+                  <a:t>הוצאות לפי חודש</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -1699,7 +3006,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>YEAR!$B$18:$M$18</c:f>
+              <c:f>YEAR!$B$34:$M$34</c:f>
               <c:strCache>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
@@ -1743,7 +3050,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>YEAR!$B$19:$M$19</c:f>
+              <c:f>YEAR!$B$38:$M$38</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -1751,7 +3058,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>230</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -1838,7 +3145,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>אוכל</a:t>
+                  <a:t>אחוז חיסכון</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -1928,6 +3235,136 @@
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -2164,6 +3601,96 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId8"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>73</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="10" name="Chart 9"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId9"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>79</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>93</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="11" name="Chart 10"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId10"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>79</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>93</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="12" name="Chart 11"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId11"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2457,7 +3984,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O36"/>
+  <dimension ref="A1:O39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -2510,10 +4037,10 @@
         <v>16</v>
       </c>
       <c r="N4" s="3" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="O4" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:15">
@@ -2527,10 +4054,10 @@
         <v>5000</v>
       </c>
       <c r="D5" s="4">
-        <v>0</v>
+        <v>4000</v>
       </c>
       <c r="E5" s="4">
-        <v>0</v>
+        <v>6000</v>
       </c>
       <c r="F5" s="4">
         <v>0</v>
@@ -2599,7 +4126,7 @@
     </row>
     <row r="8" spans="1:15">
       <c r="A8" s="3" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B8" s="5">
         <f>SUM(B5:B5)</f>
@@ -2716,27 +4243,27 @@
         <v>16</v>
       </c>
       <c r="N18" s="3" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="O18" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
     </row>
     <row r="19" spans="1:15">
       <c r="A19" s="3" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B19" s="4">
         <v>0</v>
       </c>
       <c r="C19" s="4">
-        <v>230</v>
+        <v>0</v>
       </c>
       <c r="D19" s="4">
         <v>0</v>
       </c>
       <c r="E19" s="4">
-        <v>0</v>
+        <v>520</v>
       </c>
       <c r="F19" s="4">
         <v>0</v>
@@ -2772,95 +4299,149 @@
       </c>
     </row>
     <row r="20" spans="1:15">
-      <c r="B20" s="4"/>
-      <c r="C20" s="4"/>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
-      <c r="F20" s="4"/>
-      <c r="G20" s="4"/>
-      <c r="H20" s="4"/>
-      <c r="I20" s="4"/>
-      <c r="J20" s="4"/>
-      <c r="K20" s="4"/>
-      <c r="L20" s="4"/>
-      <c r="M20" s="4"/>
+      <c r="A20" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B20" s="4">
+        <v>0</v>
+      </c>
+      <c r="C20" s="4">
+        <v>0</v>
+      </c>
+      <c r="D20" s="4">
+        <v>0</v>
+      </c>
+      <c r="E20" s="4">
+        <v>25</v>
+      </c>
+      <c r="F20" s="4">
+        <v>0</v>
+      </c>
+      <c r="G20" s="4">
+        <v>0</v>
+      </c>
+      <c r="H20" s="4">
+        <v>0</v>
+      </c>
+      <c r="I20" s="4">
+        <v>0</v>
+      </c>
+      <c r="J20" s="4">
+        <v>0</v>
+      </c>
+      <c r="K20" s="4">
+        <v>0</v>
+      </c>
+      <c r="L20" s="4">
+        <v>0</v>
+      </c>
+      <c r="M20" s="4">
+        <v>0</v>
+      </c>
+      <c r="N20" s="5">
+        <f>SUM(B20:M20)</f>
+        <v>0</v>
+      </c>
+      <c r="O20" s="5">
+        <f>AVERAGE(B20:M20)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="21" spans="1:15">
-      <c r="B21" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C21" s="6"/>
-      <c r="D21" s="6"/>
-      <c r="E21" s="6"/>
-      <c r="F21" s="6"/>
-      <c r="G21" s="6"/>
-      <c r="H21" s="6"/>
-      <c r="I21" s="6"/>
-      <c r="J21" s="6"/>
-      <c r="K21" s="6"/>
-      <c r="L21" s="6"/>
-      <c r="M21" s="6"/>
-      <c r="N21" s="6"/>
-      <c r="O21" s="6"/>
+      <c r="A21" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B21" s="4">
+        <v>0</v>
+      </c>
+      <c r="C21" s="4">
+        <v>230</v>
+      </c>
+      <c r="D21" s="4">
+        <v>230</v>
+      </c>
+      <c r="E21" s="4">
+        <v>230</v>
+      </c>
+      <c r="F21" s="4">
+        <v>0</v>
+      </c>
+      <c r="G21" s="4">
+        <v>0</v>
+      </c>
+      <c r="H21" s="4">
+        <v>0</v>
+      </c>
+      <c r="I21" s="4">
+        <v>0</v>
+      </c>
+      <c r="J21" s="4">
+        <v>0</v>
+      </c>
+      <c r="K21" s="4">
+        <v>0</v>
+      </c>
+      <c r="L21" s="4">
+        <v>0</v>
+      </c>
+      <c r="M21" s="4">
+        <v>0</v>
+      </c>
+      <c r="N21" s="5">
+        <f>SUM(B21:M21)</f>
+        <v>0</v>
+      </c>
+      <c r="O21" s="5">
+        <f>AVERAGE(B21:M21)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="22" spans="1:15">
       <c r="A22" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B22" s="5">
-        <f>SUM(B5:B5)</f>
-        <v>0</v>
-      </c>
-      <c r="C22" s="5">
-        <f>SUM(C5:C5)</f>
-        <v>0</v>
-      </c>
-      <c r="D22" s="5">
-        <f>SUM(D5:D5)</f>
-        <v>0</v>
-      </c>
-      <c r="E22" s="5">
-        <f>SUM(E5:E5)</f>
-        <v>0</v>
-      </c>
-      <c r="F22" s="5">
-        <f>SUM(F5:F5)</f>
-        <v>0</v>
-      </c>
-      <c r="G22" s="5">
-        <f>SUM(G5:G5)</f>
-        <v>0</v>
-      </c>
-      <c r="H22" s="5">
-        <f>SUM(H5:H5)</f>
-        <v>0</v>
-      </c>
-      <c r="I22" s="5">
-        <f>SUM(I5:I5)</f>
-        <v>0</v>
-      </c>
-      <c r="J22" s="5">
-        <f>SUM(J5:J5)</f>
-        <v>0</v>
-      </c>
-      <c r="K22" s="5">
-        <f>SUM(K5:K5)</f>
-        <v>0</v>
-      </c>
-      <c r="L22" s="5">
-        <f>SUM(L5:L5)</f>
-        <v>0</v>
-      </c>
-      <c r="M22" s="5">
-        <f>SUM(M5:M5)</f>
+        <v>25</v>
+      </c>
+      <c r="B22" s="4">
+        <v>0</v>
+      </c>
+      <c r="C22" s="4">
+        <v>0</v>
+      </c>
+      <c r="D22" s="4">
+        <v>0</v>
+      </c>
+      <c r="E22" s="4">
+        <v>540</v>
+      </c>
+      <c r="F22" s="4">
+        <v>0</v>
+      </c>
+      <c r="G22" s="4">
+        <v>0</v>
+      </c>
+      <c r="H22" s="4">
+        <v>0</v>
+      </c>
+      <c r="I22" s="4">
+        <v>0</v>
+      </c>
+      <c r="J22" s="4">
+        <v>0</v>
+      </c>
+      <c r="K22" s="4">
+        <v>0</v>
+      </c>
+      <c r="L22" s="4">
+        <v>0</v>
+      </c>
+      <c r="M22" s="4">
         <v>0</v>
       </c>
       <c r="N22" s="5">
-        <f>SUM(N5:N5)</f>
+        <f>SUM(B22:M22)</f>
         <v>0</v>
       </c>
       <c r="O22" s="5">
-        <f>SUM(O5:O5)</f>
+        <f>AVERAGE(B22:M22)</f>
         <v>0</v>
       </c>
     </row>
@@ -2878,325 +4459,418 @@
       <c r="L23" s="4"/>
       <c r="M23" s="4"/>
     </row>
-    <row r="28" spans="1:15">
-      <c r="A28" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B28" s="1"/>
+    <row r="24" spans="1:15">
+      <c r="B24" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C24" s="6"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="6"/>
+      <c r="F24" s="6"/>
+      <c r="G24" s="6"/>
+      <c r="H24" s="6"/>
+      <c r="I24" s="6"/>
+      <c r="J24" s="6"/>
+      <c r="K24" s="6"/>
+      <c r="L24" s="6"/>
+      <c r="M24" s="6"/>
+      <c r="N24" s="6"/>
+      <c r="O24" s="6"/>
+    </row>
+    <row r="25" spans="1:15">
+      <c r="A25" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B25" s="5">
+        <f>SUM(B19:B22)</f>
+        <v>0</v>
+      </c>
+      <c r="C25" s="5">
+        <f>SUM(C19:C22)</f>
+        <v>0</v>
+      </c>
+      <c r="D25" s="5">
+        <f>SUM(D19:D22)</f>
+        <v>0</v>
+      </c>
+      <c r="E25" s="5">
+        <f>SUM(E19:E22)</f>
+        <v>0</v>
+      </c>
+      <c r="F25" s="5">
+        <f>SUM(F19:F22)</f>
+        <v>0</v>
+      </c>
+      <c r="G25" s="5">
+        <f>SUM(G19:G22)</f>
+        <v>0</v>
+      </c>
+      <c r="H25" s="5">
+        <f>SUM(H19:H22)</f>
+        <v>0</v>
+      </c>
+      <c r="I25" s="5">
+        <f>SUM(I19:I22)</f>
+        <v>0</v>
+      </c>
+      <c r="J25" s="5">
+        <f>SUM(J19:J22)</f>
+        <v>0</v>
+      </c>
+      <c r="K25" s="5">
+        <f>SUM(K19:K22)</f>
+        <v>0</v>
+      </c>
+      <c r="L25" s="5">
+        <f>SUM(L19:L22)</f>
+        <v>0</v>
+      </c>
+      <c r="M25" s="5">
+        <f>SUM(M19:M22)</f>
+        <v>0</v>
+      </c>
+      <c r="N25" s="5">
+        <f>SUM(N19:N22)</f>
+        <v>0</v>
+      </c>
+      <c r="O25" s="5">
+        <f>SUM(O19:O22)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15">
+      <c r="B26" s="4"/>
+      <c r="C26" s="4"/>
+      <c r="D26" s="4"/>
+      <c r="E26" s="4"/>
+      <c r="F26" s="4"/>
+      <c r="G26" s="4"/>
+      <c r="H26" s="4"/>
+      <c r="I26" s="4"/>
+      <c r="J26" s="4"/>
+      <c r="K26" s="4"/>
+      <c r="L26" s="4"/>
+      <c r="M26" s="4"/>
     </row>
     <row r="31" spans="1:15">
-      <c r="A31" s="4"/>
-      <c r="B31" s="3" t="s">
+      <c r="A31" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B31" s="1"/>
+    </row>
+    <row r="34" spans="1:15">
+      <c r="A34" s="4"/>
+      <c r="B34" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C31" s="3" t="s">
+      <c r="C34" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D31" s="3" t="s">
+      <c r="D34" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E31" s="3" t="s">
+      <c r="E34" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="F31" s="3" t="s">
+      <c r="F34" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="G31" s="3" t="s">
+      <c r="G34" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="H31" s="3" t="s">
+      <c r="H34" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="I31" s="3" t="s">
+      <c r="I34" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="J31" s="3" t="s">
+      <c r="J34" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="K31" s="3" t="s">
+      <c r="K34" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="L31" s="3" t="s">
+      <c r="L34" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="M31" s="3" t="s">
+      <c r="M34" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="N31" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="O31" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="32" spans="1:15">
-      <c r="A32" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B32" s="5">
-        <f>B8</f>
-        <v>0</v>
-      </c>
-      <c r="C32" s="5">
-        <f>C8</f>
-        <v>0</v>
-      </c>
-      <c r="D32" s="5">
-        <f>D8</f>
-        <v>0</v>
-      </c>
-      <c r="E32" s="5">
-        <f>E8</f>
-        <v>0</v>
-      </c>
-      <c r="F32" s="5">
-        <f>F8</f>
-        <v>0</v>
-      </c>
-      <c r="G32" s="5">
-        <f>G8</f>
-        <v>0</v>
-      </c>
-      <c r="H32" s="5">
-        <f>H8</f>
-        <v>0</v>
-      </c>
-      <c r="I32" s="5">
-        <f>I8</f>
-        <v>0</v>
-      </c>
-      <c r="J32" s="5">
-        <f>J8</f>
-        <v>0</v>
-      </c>
-      <c r="K32" s="5">
-        <f>K8</f>
-        <v>0</v>
-      </c>
-      <c r="L32" s="5">
-        <f>L8</f>
-        <v>0</v>
-      </c>
-      <c r="M32" s="5">
-        <f>M8</f>
-        <v>0</v>
-      </c>
-      <c r="N32" s="5">
-        <f>N8</f>
-        <v>0</v>
-      </c>
-      <c r="O32" s="5">
-        <f>O8</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:15">
-      <c r="A33" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B33" s="5">
-        <f>B22</f>
-        <v>0</v>
-      </c>
-      <c r="C33" s="5">
-        <f>C22</f>
-        <v>0</v>
-      </c>
-      <c r="D33" s="5">
-        <f>D22</f>
-        <v>0</v>
-      </c>
-      <c r="E33" s="5">
-        <f>E22</f>
-        <v>0</v>
-      </c>
-      <c r="F33" s="5">
-        <f>F22</f>
-        <v>0</v>
-      </c>
-      <c r="G33" s="5">
-        <f>G22</f>
-        <v>0</v>
-      </c>
-      <c r="H33" s="5">
-        <f>H22</f>
-        <v>0</v>
-      </c>
-      <c r="I33" s="5">
-        <f>I22</f>
-        <v>0</v>
-      </c>
-      <c r="J33" s="5">
-        <f>J22</f>
-        <v>0</v>
-      </c>
-      <c r="K33" s="5">
-        <f>K22</f>
-        <v>0</v>
-      </c>
-      <c r="L33" s="5">
-        <f>L22</f>
-        <v>0</v>
-      </c>
-      <c r="M33" s="5">
-        <f>M22</f>
-        <v>0</v>
-      </c>
-      <c r="N33" s="5">
-        <f>N22</f>
-        <v>0</v>
-      </c>
-      <c r="O33" s="5">
-        <f>O22</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:15">
-      <c r="A34" s="3" t="s">
+      <c r="N34" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="O34" s="3" t="s">
         <v>27</v>
-      </c>
-      <c r="B34" s="5">
-        <f>B8-B22</f>
-        <v>0</v>
-      </c>
-      <c r="C34" s="5">
-        <f>C8-C22</f>
-        <v>0</v>
-      </c>
-      <c r="D34" s="5">
-        <f>D8-D22</f>
-        <v>0</v>
-      </c>
-      <c r="E34" s="5">
-        <f>E8-E22</f>
-        <v>0</v>
-      </c>
-      <c r="F34" s="5">
-        <f>F8-F22</f>
-        <v>0</v>
-      </c>
-      <c r="G34" s="5">
-        <f>G8-G22</f>
-        <v>0</v>
-      </c>
-      <c r="H34" s="5">
-        <f>H8-H22</f>
-        <v>0</v>
-      </c>
-      <c r="I34" s="5">
-        <f>I8-I22</f>
-        <v>0</v>
-      </c>
-      <c r="J34" s="5">
-        <f>J8-J22</f>
-        <v>0</v>
-      </c>
-      <c r="K34" s="5">
-        <f>K8-K22</f>
-        <v>0</v>
-      </c>
-      <c r="L34" s="5">
-        <f>L8-L22</f>
-        <v>0</v>
-      </c>
-      <c r="M34" s="5">
-        <f>M8-M22</f>
-        <v>0</v>
-      </c>
-      <c r="N34" s="5">
-        <f>N8-N22</f>
-        <v>0</v>
-      </c>
-      <c r="O34" s="5">
-        <f>O8-O22</f>
-        <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:15">
       <c r="A35" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B35" s="7">
-        <f>IFERROR(B34/B8, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="C35" s="7">
-        <f>IFERROR(C34/C8, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="D35" s="7">
-        <f>IFERROR(D34/D8, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="E35" s="7">
-        <f>IFERROR(E34/E8, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="F35" s="7">
-        <f>IFERROR(F34/F8, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="G35" s="7">
-        <f>IFERROR(G34/G8, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="H35" s="7">
-        <f>IFERROR(H34/H8, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="I35" s="7">
-        <f>IFERROR(I34/I8, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="J35" s="7">
-        <f>IFERROR(J34/J8, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="K35" s="7">
-        <f>IFERROR(K34/K8, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="L35" s="7">
-        <f>IFERROR(L34/L8, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="M35" s="7">
-        <f>IFERROR(M34/M8, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="N35" s="7">
-        <f>IFERROR(N34/N8, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="O35" s="7">
-        <f>IFERROR(O34/O8, 0)</f>
+        <v>19</v>
+      </c>
+      <c r="B35" s="5">
+        <f>B8</f>
+        <v>0</v>
+      </c>
+      <c r="C35" s="5">
+        <f>C8</f>
+        <v>0</v>
+      </c>
+      <c r="D35" s="5">
+        <f>D8</f>
+        <v>0</v>
+      </c>
+      <c r="E35" s="5">
+        <f>E8</f>
+        <v>0</v>
+      </c>
+      <c r="F35" s="5">
+        <f>F8</f>
+        <v>0</v>
+      </c>
+      <c r="G35" s="5">
+        <f>G8</f>
+        <v>0</v>
+      </c>
+      <c r="H35" s="5">
+        <f>H8</f>
+        <v>0</v>
+      </c>
+      <c r="I35" s="5">
+        <f>I8</f>
+        <v>0</v>
+      </c>
+      <c r="J35" s="5">
+        <f>J8</f>
+        <v>0</v>
+      </c>
+      <c r="K35" s="5">
+        <f>K8</f>
+        <v>0</v>
+      </c>
+      <c r="L35" s="5">
+        <f>L8</f>
+        <v>0</v>
+      </c>
+      <c r="M35" s="5">
+        <f>M8</f>
+        <v>0</v>
+      </c>
+      <c r="N35" s="5">
+        <f>N8</f>
+        <v>0</v>
+      </c>
+      <c r="O35" s="5">
+        <f>O8</f>
         <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:15">
-      <c r="A36" s="4"/>
-      <c r="B36" s="4"/>
-      <c r="C36" s="4"/>
-      <c r="D36" s="4"/>
-      <c r="E36" s="4"/>
-      <c r="F36" s="4"/>
-      <c r="G36" s="4"/>
-      <c r="H36" s="4"/>
-      <c r="I36" s="4"/>
-      <c r="J36" s="4"/>
-      <c r="K36" s="4"/>
-      <c r="L36" s="4"/>
-      <c r="M36" s="4"/>
-      <c r="N36" s="4"/>
-      <c r="O36" s="4"/>
+      <c r="A36" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B36" s="5">
+        <f>B25</f>
+        <v>0</v>
+      </c>
+      <c r="C36" s="5">
+        <f>C25</f>
+        <v>0</v>
+      </c>
+      <c r="D36" s="5">
+        <f>D25</f>
+        <v>0</v>
+      </c>
+      <c r="E36" s="5">
+        <f>E25</f>
+        <v>0</v>
+      </c>
+      <c r="F36" s="5">
+        <f>F25</f>
+        <v>0</v>
+      </c>
+      <c r="G36" s="5">
+        <f>G25</f>
+        <v>0</v>
+      </c>
+      <c r="H36" s="5">
+        <f>H25</f>
+        <v>0</v>
+      </c>
+      <c r="I36" s="5">
+        <f>I25</f>
+        <v>0</v>
+      </c>
+      <c r="J36" s="5">
+        <f>J25</f>
+        <v>0</v>
+      </c>
+      <c r="K36" s="5">
+        <f>K25</f>
+        <v>0</v>
+      </c>
+      <c r="L36" s="5">
+        <f>L25</f>
+        <v>0</v>
+      </c>
+      <c r="M36" s="5">
+        <f>M25</f>
+        <v>0</v>
+      </c>
+      <c r="N36" s="5">
+        <f>N25</f>
+        <v>0</v>
+      </c>
+      <c r="O36" s="5">
+        <f>O25</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15">
+      <c r="A37" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B37" s="5">
+        <f>B8-B25</f>
+        <v>0</v>
+      </c>
+      <c r="C37" s="5">
+        <f>C8-C25</f>
+        <v>0</v>
+      </c>
+      <c r="D37" s="5">
+        <f>D8-D25</f>
+        <v>0</v>
+      </c>
+      <c r="E37" s="5">
+        <f>E8-E25</f>
+        <v>0</v>
+      </c>
+      <c r="F37" s="5">
+        <f>F8-F25</f>
+        <v>0</v>
+      </c>
+      <c r="G37" s="5">
+        <f>G8-G25</f>
+        <v>0</v>
+      </c>
+      <c r="H37" s="5">
+        <f>H8-H25</f>
+        <v>0</v>
+      </c>
+      <c r="I37" s="5">
+        <f>I8-I25</f>
+        <v>0</v>
+      </c>
+      <c r="J37" s="5">
+        <f>J8-J25</f>
+        <v>0</v>
+      </c>
+      <c r="K37" s="5">
+        <f>K8-K25</f>
+        <v>0</v>
+      </c>
+      <c r="L37" s="5">
+        <f>L8-L25</f>
+        <v>0</v>
+      </c>
+      <c r="M37" s="5">
+        <f>M8-M25</f>
+        <v>0</v>
+      </c>
+      <c r="N37" s="5">
+        <f>N8-N25</f>
+        <v>0</v>
+      </c>
+      <c r="O37" s="5">
+        <f>O8-O25</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15">
+      <c r="A38" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B38" s="7">
+        <f>IFERROR(B37/B8, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="C38" s="7">
+        <f>IFERROR(C37/C8, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="D38" s="7">
+        <f>IFERROR(D37/D8, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="E38" s="7">
+        <f>IFERROR(E37/E8, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="F38" s="7">
+        <f>IFERROR(F37/F8, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="G38" s="7">
+        <f>IFERROR(G37/G8, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="H38" s="7">
+        <f>IFERROR(H37/H8, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="I38" s="7">
+        <f>IFERROR(I37/I8, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="J38" s="7">
+        <f>IFERROR(J37/J8, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="K38" s="7">
+        <f>IFERROR(K37/K8, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="L38" s="7">
+        <f>IFERROR(L37/L8, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="M38" s="7">
+        <f>IFERROR(M37/M8, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="N38" s="7">
+        <f>IFERROR(N37/N8, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="O38" s="7">
+        <f>IFERROR(O37/O8, 0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15">
+      <c r="A39" s="4"/>
+      <c r="B39" s="4"/>
+      <c r="C39" s="4"/>
+      <c r="D39" s="4"/>
+      <c r="E39" s="4"/>
+      <c r="F39" s="4"/>
+      <c r="G39" s="4"/>
+      <c r="H39" s="4"/>
+      <c r="I39" s="4"/>
+      <c r="J39" s="4"/>
+      <c r="K39" s="4"/>
+      <c r="L39" s="4"/>
+      <c r="M39" s="4"/>
+      <c r="N39" s="4"/>
+      <c r="O39" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="B7:O7"/>
     <mergeCell ref="A15:B15"/>
-    <mergeCell ref="B21:O21"/>
-    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="B24:O24"/>
+    <mergeCell ref="A31:B31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3816,7 +5490,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N10"/>
+  <dimension ref="A1:N11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3864,65 +5538,83 @@
       <c r="K4" s="3"/>
     </row>
     <row r="5" spans="1:14">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="4">
+        <v>230</v>
+      </c>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="H5" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I5" s="4">
+        <v>4000</v>
+      </c>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+    </row>
+    <row r="6" spans="1:14">
+      <c r="A6" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="6"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="H5" s="6" t="s">
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="H6" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="I5" s="6"/>
-      <c r="J5" s="6"/>
-      <c r="K5" s="6"/>
-    </row>
-    <row r="6" spans="1:14">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-      <c r="J6" s="3"/>
-      <c r="K6" s="3"/>
+      <c r="I6" s="6"/>
+      <c r="J6" s="6"/>
+      <c r="K6" s="6"/>
     </row>
     <row r="7" spans="1:14">
-      <c r="A7" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B7" s="4">
-        <f>SUM(B5:B4)</f>
-        <v>0</v>
-      </c>
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
-      <c r="H7" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="I7" s="4">
-        <f>SUM(I5:I4)</f>
-        <v>0</v>
-      </c>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
       <c r="J7" s="3"/>
       <c r="K7" s="3"/>
     </row>
     <row r="8" spans="1:14">
-      <c r="A8" s="3"/>
-      <c r="B8" s="3"/>
+      <c r="A8" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="4">
+        <f>SUM(B5:B5)</f>
+        <v>0</v>
+      </c>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
+      <c r="H8" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="I8" s="4">
+        <f>SUM(I5:I5)</f>
+        <v>0</v>
+      </c>
       <c r="J8" s="3"/>
       <c r="K8" s="3"/>
     </row>
-    <row r="10" spans="1:14">
-      <c r="H10" s="5" t="s">
+    <row r="9" spans="1:14">
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
+      <c r="K9" s="3"/>
+    </row>
+    <row r="11" spans="1:14">
+      <c r="H11" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="I10" s="5">
-        <f>SUM(-B7, I7)</f>
+      <c r="I11" s="5">
+        <f>SUM(-B8, I8)</f>
         <v>0</v>
       </c>
     </row>
@@ -3930,16 +5622,17 @@
   <mergeCells count="4">
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="H1:I1"/>
-    <mergeCell ref="A5:D5"/>
-    <mergeCell ref="H5:K5"/>
+    <mergeCell ref="A6:D6"/>
+    <mergeCell ref="H6:K6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N10"/>
+  <dimension ref="A1:N12"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3987,76 +5680,123 @@
       <c r="K4" s="3"/>
     </row>
     <row r="5" spans="1:14">
-      <c r="A5" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="B5" s="6"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="H5" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="I5" s="6"/>
-      <c r="J5" s="6"/>
-      <c r="K5" s="6"/>
+      <c r="A5" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="4">
+        <v>520</v>
+      </c>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="H5" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I5" s="4">
+        <v>6000</v>
+      </c>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
     </row>
     <row r="6" spans="1:14">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
+      <c r="A6" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" s="4">
+        <v>25</v>
+      </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-      <c r="J6" s="3"/>
-      <c r="K6" s="3"/>
+      <c r="H6" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="I6" s="6"/>
+      <c r="J6" s="6"/>
+      <c r="K6" s="6"/>
     </row>
     <row r="7" spans="1:14">
       <c r="A7" s="3" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="B7" s="4">
-        <f>SUM(B5:B4)</f>
-        <v>0</v>
+        <v>540</v>
       </c>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
-      <c r="H7" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="I7" s="4">
-        <f>SUM(I5:I4)</f>
-        <v>0</v>
-      </c>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
       <c r="J7" s="3"/>
       <c r="K7" s="3"/>
     </row>
     <row r="8" spans="1:14">
-      <c r="A8" s="3"/>
-      <c r="B8" s="3"/>
+      <c r="A8" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="4">
+        <v>230</v>
+      </c>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
+      <c r="H8" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="I8" s="4">
+        <f>SUM(I5:I5)</f>
+        <v>0</v>
+      </c>
       <c r="J8" s="3"/>
       <c r="K8" s="3"/>
     </row>
+    <row r="9" spans="1:14">
+      <c r="A9" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="6"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
+      <c r="K9" s="3"/>
+    </row>
     <row r="10" spans="1:14">
-      <c r="H10" s="5" t="s">
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+    </row>
+    <row r="11" spans="1:14">
+      <c r="A11" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="4">
+        <f>SUM(B5:B8)</f>
+        <v>0</v>
+      </c>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="H11" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="I10" s="5">
-        <f>SUM(-B7, I7)</f>
-        <v>0</v>
-      </c>
+      <c r="I11" s="5">
+        <f>SUM(-B11, I8)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14">
+      <c r="A12" s="3"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="H1:I1"/>
-    <mergeCell ref="A5:D5"/>
-    <mergeCell ref="H5:K5"/>
+    <mergeCell ref="A9:D9"/>
+    <mergeCell ref="H6:K6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>